<commit_message>
Added evaluation for 3 constellations.
</commit_message>
<xml_diff>
--- a/thesis_data/evaluation_data/evaluation_data.xlsx
+++ b/thesis_data/evaluation_data/evaluation_data.xlsx
@@ -7,16 +7,17 @@
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet name="cancer" sheetId="1" r:id="rId1"/>
-    <sheet name="lepus" sheetId="2" r:id="rId2"/>
-    <sheet name="aries" sheetId="3" r:id="rId3"/>
+    <sheet name="aries" sheetId="5" r:id="rId1"/>
+    <sheet name="lepus" sheetId="4" r:id="rId2"/>
+    <sheet name="cancer" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="16">
   <si>
     <t>Total</t>
   </si>
@@ -39,15 +40,6 @@
     <t>sample size</t>
   </si>
   <si>
-    <t>triangles_difference_threshold</t>
-  </si>
-  <si>
-    <t>area_threshold</t>
-  </si>
-  <si>
-    <t>position_variation</t>
-  </si>
-  <si>
     <t>triangles difference threshold</t>
   </si>
   <si>
@@ -57,10 +49,22 @@
     <t>position variation from center</t>
   </si>
   <si>
-    <t>losses due to position variaton from center</t>
+    <t>lepus</t>
   </si>
   <si>
-    <t>losses due to area threshold</t>
+    <t>false detections</t>
+  </si>
+  <si>
+    <t>false detections due to position variaton from center</t>
+  </si>
+  <si>
+    <t>false detections due to area threshold</t>
+  </si>
+  <si>
+    <t>aries</t>
+  </si>
+  <si>
+    <t>11 w/ 1 false detection</t>
   </si>
 </sst>
 </file>
@@ -399,11 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,13 +429,13 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -446,7 +449,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>0.01</v>
@@ -458,11 +461,11 @@
         <v>3</v>
       </c>
       <c r="F2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G2">
         <f>(F2/H2)</f>
-        <v>0.3</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="H2">
         <v>30</v>
@@ -470,7 +473,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>0.01</v>
@@ -482,11 +485,11 @@
         <v>5</v>
       </c>
       <c r="F3">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G13" si="0">(F3/H3)</f>
-        <v>0.4</v>
+        <f t="shared" ref="G3:G18" si="0">(F3/H3)</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="H3">
         <v>30</v>
@@ -494,7 +497,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>0.05</v>
@@ -505,12 +508,12 @@
       <c r="E4">
         <v>5</v>
       </c>
-      <c r="F4">
-        <v>25</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="0"/>
-        <v>0.83333333333333337</v>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
       </c>
       <c r="H4">
         <v>30</v>
@@ -518,7 +521,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>0.05</v>
@@ -529,12 +532,12 @@
       <c r="E5">
         <v>3</v>
       </c>
-      <c r="F5">
-        <v>13</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>0.43333333333333335</v>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
       </c>
       <c r="H5">
         <v>30</v>
@@ -542,7 +545,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>0.01</v>
@@ -554,11 +557,11 @@
         <v>3</v>
       </c>
       <c r="F6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="H6">
         <v>30</v>
@@ -566,7 +569,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>0.01</v>
@@ -578,11 +581,11 @@
         <v>5</v>
       </c>
       <c r="F7">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>0.43333333333333335</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="H7">
         <v>30</v>
@@ -590,7 +593,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>0.05</v>
@@ -601,12 +604,12 @@
       <c r="E8">
         <v>5</v>
       </c>
-      <c r="F8">
-        <v>26</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>0.8666666666666667</v>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
       </c>
       <c r="H8">
         <v>30</v>
@@ -614,7 +617,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>0.05</v>
@@ -625,12 +628,12 @@
       <c r="E9">
         <v>3</v>
       </c>
-      <c r="F9">
-        <v>14</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>0.46666666666666667</v>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
       </c>
       <c r="H9">
         <v>30</v>
@@ -638,7 +641,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>0.05</v>
@@ -650,7 +653,7 @@
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G10" t="e">
         <f t="shared" si="0"/>
@@ -662,7 +665,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>0.05</v>
@@ -674,7 +677,7 @@
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G11" t="e">
         <f t="shared" si="0"/>
@@ -686,11 +689,23 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>0.03</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
       </c>
       <c r="H12">
         <v>30</v>
@@ -698,13 +713,145 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>0.03</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
       </c>
       <c r="H13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>0.03</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>0.03</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>0.02</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>0.02</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>0.02</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H18">
         <v>30</v>
       </c>
     </row>
@@ -718,7 +865,7 @@
       </c>
       <c r="F53">
         <f>SUM(F2:F50)</f>
-        <v>122</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -729,44 +876,792 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:D1"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.5546875" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="30.21875" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>0.01</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>19</v>
+      </c>
+      <c r="G2">
+        <f>(F2/H2)</f>
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>0.01</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>24</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G13" si="0">(F3/H3)</f>
+        <v>0.8</v>
+      </c>
+      <c r="H3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>0.05</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>0.05</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>0.01</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>19</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="H6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>0.01</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>24</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="H7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>0.05</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>0.05</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>0.05</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>0.05</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>0.03</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>0.03</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>20</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>0.03</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>0.03</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53">
+        <f>SUM(B2:B50)</f>
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <f>SUM(F2:F50)</f>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:H53"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="30.21875" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="18.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>0.01</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>9</v>
+      </c>
+      <c r="G2">
+        <f>(F2/H2)</f>
+        <v>0.3</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>0.01</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>12</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G15" si="0">(F3/H3)</f>
+        <v>0.4</v>
+      </c>
+      <c r="H3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>0.05</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>25</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>0.05</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="H5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0.01</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>0.01</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>13</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="H7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>0.05</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>26</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="H8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>0.05</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="H9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>0.05</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>0.05</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>0.03</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>0.03</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="H13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>0.03</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>21</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="H14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>0.03</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="H15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53">
+        <f>SUM(B2:B50)</f>
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <f>SUM(F2:F50)</f>
+        <v>190</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>

<commit_message>
Added feature to evaluation: if a set of matching points has a lower luminosity than any other set already found, it is not considered. Improved the accuracy.
</commit_message>
<xml_diff>
--- a/thesis_data/evaluation_data/evaluation_data.xlsx
+++ b/thesis_data/evaluation_data/evaluation_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -390,16 +390,16 @@
   <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="13.77734375" style="1" customWidth="1"/>
-    <col min="9" max="10" width="13.77734375" customWidth="1"/>
+    <col min="1" max="8" width="13.7109375" style="1" customWidth="1"/>
+    <col min="9" max="10" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -431,34 +431,34 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="C2" s="1">
         <v>3</v>
       </c>
       <c r="D2" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1">
         <v>10</v>
       </c>
       <c r="F2" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1">
         <v>10</v>
       </c>
       <c r="H2" s="1">
         <f>F2/G2</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>1</v>
@@ -471,7 +471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A67" si="0">A3+1</f>
         <v>2</v>
@@ -499,33 +499,63 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
+      <c r="B5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>7</v>
+      </c>
       <c r="G5" s="1">
         <v>10</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
+      <c r="B6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6</v>
+      </c>
       <c r="G6" s="1">
         <v>10</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -538,7 +568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -551,7 +581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -564,7 +594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -577,7 +607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -590,7 +620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -603,7 +633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -616,7 +646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -629,7 +659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -642,7 +672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -655,7 +685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -668,7 +698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -681,7 +711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -694,7 +724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -707,7 +737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -720,7 +750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -733,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -746,7 +776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -759,7 +789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -772,7 +802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -785,7 +815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -798,7 +828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -811,7 +841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -824,7 +854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -837,7 +867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -850,7 +880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -863,7 +893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -876,7 +906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -889,7 +919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -902,7 +932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -915,7 +945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -928,7 +958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -941,7 +971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -954,7 +984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -967,7 +997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -980,7 +1010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -993,7 +1023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1006,7 +1036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1019,7 +1049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1032,7 +1062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1045,7 +1075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1058,7 +1088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1071,7 +1101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1084,7 +1114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -1097,7 +1127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -1110,7 +1140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -1123,7 +1153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -1136,7 +1166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -1149,7 +1179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -1162,7 +1192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -1175,7 +1205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -1188,7 +1218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -1201,7 +1231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -1214,7 +1244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -1227,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -1240,7 +1270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -1253,7 +1283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -1266,7 +1296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -1279,7 +1309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -1292,7 +1322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -1305,7 +1335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -1318,9 +1348,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <f t="shared" ref="A68:A92" si="2">A67+1</f>
+        <f t="shared" ref="A68:A91" si="2">A67+1</f>
         <v>66</v>
       </c>
       <c r="G68" s="1">
@@ -1331,7 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <f t="shared" si="2"/>
         <v>67</v>
@@ -1344,7 +1374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <f t="shared" si="2"/>
         <v>68</v>
@@ -1357,7 +1387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <f t="shared" si="2"/>
         <v>69</v>
@@ -1370,7 +1400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <f t="shared" si="2"/>
         <v>70</v>
@@ -1383,7 +1413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <f t="shared" si="2"/>
         <v>71</v>
@@ -1396,7 +1426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <f t="shared" si="2"/>
         <v>72</v>
@@ -1409,7 +1439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <f t="shared" si="2"/>
         <v>73</v>
@@ -1422,7 +1452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <f t="shared" si="2"/>
         <v>74</v>
@@ -1435,7 +1465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <f t="shared" si="2"/>
         <v>75</v>
@@ -1448,7 +1478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <f t="shared" si="2"/>
         <v>76</v>
@@ -1461,7 +1491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <f t="shared" si="2"/>
         <v>77</v>
@@ -1474,7 +1504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <f t="shared" si="2"/>
         <v>78</v>
@@ -1487,7 +1517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <f t="shared" si="2"/>
         <v>79</v>
@@ -1500,7 +1530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <f t="shared" si="2"/>
         <v>80</v>
@@ -1513,7 +1543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <f t="shared" si="2"/>
         <v>81</v>
@@ -1526,7 +1556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <f t="shared" si="2"/>
         <v>82</v>
@@ -1539,7 +1569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <f t="shared" si="2"/>
         <v>83</v>
@@ -1552,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <f t="shared" si="2"/>
         <v>84</v>
@@ -1565,7 +1595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <f t="shared" si="2"/>
         <v>85</v>
@@ -1578,7 +1608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <f t="shared" si="2"/>
         <v>86</v>
@@ -1591,7 +1621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <f t="shared" si="2"/>
         <v>87</v>
@@ -1604,7 +1634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <f t="shared" si="2"/>
         <v>88</v>
@@ -1617,7 +1647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <f t="shared" si="2"/>
         <v>89</v>
@@ -1642,7 +1672,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1654,7 +1684,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added evaluation for some constellations.
</commit_message>
<xml_diff>
--- a/thesis_data/evaluation_data/evaluation_data.xlsx
+++ b/thesis_data/evaluation_data/evaluation_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>constellation nb</t>
   </si>
@@ -42,10 +42,31 @@
     <t>success rate</t>
   </si>
   <si>
-    <t>status</t>
+    <t>3 or 5</t>
   </si>
   <si>
-    <t>reason</t>
+    <t>solved with</t>
+  </si>
+  <si>
+    <t>multiple det.</t>
+  </si>
+  <si>
+    <t>abbreviations</t>
+  </si>
+  <si>
+    <t>GreLum or LowDiff</t>
+  </si>
+  <si>
+    <t>LowDiff = take set with lowest triangle difference</t>
+  </si>
+  <si>
+    <t>GreLum = take set with greatest luminosity</t>
+  </si>
+  <si>
+    <t>GreLum, LowDiff</t>
+  </si>
+  <si>
+    <t>GreLum, LowDiff. Remove some stars from model for better results?</t>
   </si>
 </sst>
 </file>
@@ -81,9 +102,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -387,19 +411,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J91"/>
+  <dimension ref="A1:K91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="13.7109375" style="1" customWidth="1"/>
-    <col min="9" max="10" width="13.7109375" customWidth="1"/>
+    <col min="1" max="5" width="13.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="1" customWidth="1"/>
+    <col min="7" max="8" width="13.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="34.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -425,13 +453,16 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -442,7 +473,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1">
         <v>10</v>
@@ -457,8 +488,17 @@
         <f>F2/G2</f>
         <v>0.9</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>1</v>
@@ -470,8 +510,11 @@
         <f>F3/G3</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A67" si="0">A3+1</f>
         <v>2</v>
@@ -498,8 +541,11 @@
         <f t="shared" ref="H4:H67" si="1">F4/G4</f>
         <v>0.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -526,8 +572,11 @@
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -554,99 +603,240 @@
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="B7" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1">
+        <v>10</v>
+      </c>
       <c r="G7" s="1">
         <v>10</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
+      <c r="B8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1">
+        <v>9</v>
+      </c>
       <c r="G8" s="1">
         <v>10</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+        <v>0.9</v>
+      </c>
+      <c r="I8" s="1">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
+      <c r="B9" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1">
+        <v>10</v>
+      </c>
       <c r="G9" s="1">
         <v>10</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="B10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
       <c r="G10" s="1">
         <v>10</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+        <v>0.3</v>
+      </c>
+      <c r="I10" s="1">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
+      <c r="B11" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="C11" s="1">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1">
+        <v>10</v>
+      </c>
       <c r="G11" s="1">
         <v>10</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="B12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1">
+        <v>7</v>
+      </c>
+      <c r="F12" s="1">
+        <v>8</v>
+      </c>
       <c r="G12" s="1">
         <v>10</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+        <v>0.8</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
+      <c r="B13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1">
+        <v>5</v>
+      </c>
+      <c r="E13" s="1">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1">
+        <v>30</v>
+      </c>
       <c r="G13" s="1">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -659,20 +849,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
+      <c r="B15" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>5</v>
+      </c>
+      <c r="E15" s="1">
+        <v>10</v>
+      </c>
+      <c r="F15" s="1">
+        <v>10</v>
+      </c>
       <c r="G15" s="1">
         <v>10</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -685,59 +893,134 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
+      <c r="B17" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1">
+        <v>5</v>
+      </c>
+      <c r="E17" s="1">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1">
+        <v>5</v>
+      </c>
       <c r="G17" s="1">
         <v>10</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+        <v>0.5</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
+      <c r="B18" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1">
+        <v>10</v>
+      </c>
+      <c r="F18" s="1">
+        <v>8</v>
+      </c>
       <c r="G18" s="1">
         <v>10</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+        <v>0.8</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
+      <c r="B19" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>7</v>
+      </c>
+      <c r="E19" s="1">
+        <v>10</v>
+      </c>
+      <c r="F19" s="1">
+        <v>10</v>
+      </c>
       <c r="G19" s="1">
         <v>10</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
+      <c r="B20" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1">
+        <v>7</v>
+      </c>
+      <c r="E20" s="1">
+        <v>10</v>
+      </c>
+      <c r="F20" s="1">
+        <v>2</v>
+      </c>
       <c r="G20" s="1">
         <v>10</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+        <v>0.2</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -750,7 +1033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -763,7 +1046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -776,7 +1059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -789,7 +1072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -802,7 +1085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -815,7 +1098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -828,7 +1111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -841,7 +1124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -854,7 +1137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -867,7 +1150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -880,7 +1163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>30</v>

</xml_diff>

<commit_message>
Added evaluations for constellations up to number 38.
</commit_message>
<xml_diff>
--- a/thesis_data/evaluation_data/evaluation_data.xlsx
+++ b/thesis_data/evaluation_data/evaluation_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>constellation nb</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>GreLum, LowDiff. Remove some stars from model for better results?</t>
+  </si>
+  <si>
+    <t>GreLum</t>
+  </si>
+  <si>
+    <t>some cases GreLum, some LowDiff. Hard because of only 3 stars in constellation</t>
   </si>
 </sst>
 </file>
@@ -413,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,12 +1031,33 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
+      <c r="B21" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1">
+        <v>10</v>
+      </c>
+      <c r="E21" s="1">
+        <v>10</v>
+      </c>
+      <c r="F21" s="1">
+        <v>10</v>
+      </c>
       <c r="G21" s="1">
         <v>10</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I21" s="1">
+        <v>8</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1038,12 +1065,33 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
+      <c r="B22" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>10</v>
+      </c>
+      <c r="E22" s="1">
+        <v>7</v>
+      </c>
+      <c r="F22" s="1">
+        <v>4</v>
+      </c>
       <c r="G22" s="1">
         <v>10</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.4</v>
+      </c>
+      <c r="I22" s="1">
+        <v>2</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1051,12 +1099,33 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
+      <c r="B23" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1">
+        <v>5</v>
+      </c>
+      <c r="E23" s="1">
+        <v>10</v>
+      </c>
+      <c r="F23" s="1">
+        <v>10</v>
+      </c>
       <c r="G23" s="1">
         <v>10</v>
       </c>
       <c r="H23" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I23" s="1">
+        <v>4</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1064,12 +1133,33 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
+      <c r="B24" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C24" s="1">
+        <v>3</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3</v>
+      </c>
+      <c r="E24" s="1">
+        <v>10</v>
+      </c>
+      <c r="F24" s="1">
+        <v>10</v>
+      </c>
       <c r="G24" s="1">
         <v>10</v>
       </c>
       <c r="H24" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I24" s="1">
+        <v>1</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1077,12 +1167,33 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
+      <c r="B25" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C25" s="1">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1">
+        <v>5</v>
+      </c>
+      <c r="E25" s="1">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1">
+        <v>10</v>
+      </c>
       <c r="G25" s="1">
         <v>10</v>
       </c>
       <c r="H25" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I25" s="1">
+        <v>2</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1090,12 +1201,33 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
+      <c r="B26" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C26" s="1">
+        <v>3</v>
+      </c>
+      <c r="D26" s="1">
+        <v>3</v>
+      </c>
+      <c r="E26" s="1">
+        <v>10</v>
+      </c>
+      <c r="F26" s="1">
+        <v>10</v>
+      </c>
       <c r="G26" s="1">
         <v>10</v>
       </c>
       <c r="H26" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I26" s="1">
+        <v>2</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1103,12 +1235,33 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
+      <c r="B27" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C27" s="1">
+        <v>3</v>
+      </c>
+      <c r="D27" s="1">
+        <v>5</v>
+      </c>
+      <c r="E27" s="1">
+        <v>20</v>
+      </c>
+      <c r="F27" s="1">
+        <v>6</v>
+      </c>
       <c r="G27" s="1">
         <v>10</v>
       </c>
       <c r="H27" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.6</v>
+      </c>
+      <c r="I27" s="1">
+        <v>2</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1116,11 +1269,29 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
+      <c r="B28" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C28" s="1">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1">
+        <v>3</v>
+      </c>
+      <c r="E28" s="1">
+        <v>10</v>
+      </c>
+      <c r="F28" s="1">
+        <v>10</v>
+      </c>
       <c r="G28" s="1">
         <v>10</v>
       </c>
       <c r="H28" s="1">
         <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I28" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1129,11 +1300,29 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
+      <c r="B29" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C29" s="1">
+        <v>3</v>
+      </c>
+      <c r="D29" s="1">
+        <v>3</v>
+      </c>
+      <c r="E29" s="1">
+        <v>10</v>
+      </c>
+      <c r="F29" s="1">
+        <v>10</v>
+      </c>
       <c r="G29" s="1">
         <v>10</v>
       </c>
       <c r="H29" s="1">
         <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I29" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1142,11 +1331,29 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
+      <c r="B30" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C30" s="1">
+        <v>3</v>
+      </c>
+      <c r="D30" s="1">
+        <v>3</v>
+      </c>
+      <c r="E30" s="1">
+        <v>10</v>
+      </c>
+      <c r="F30" s="1">
+        <v>10</v>
+      </c>
       <c r="G30" s="1">
         <v>10</v>
       </c>
       <c r="H30" s="1">
         <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I30" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1155,12 +1362,33 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
+      <c r="B31" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C31" s="1">
+        <v>3</v>
+      </c>
+      <c r="D31" s="1">
+        <v>3</v>
+      </c>
+      <c r="E31" s="1">
+        <v>10</v>
+      </c>
+      <c r="F31" s="1">
+        <v>10</v>
+      </c>
       <c r="G31" s="1">
         <v>10</v>
       </c>
       <c r="H31" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I31" s="1">
+        <v>2</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1168,54 +1396,132 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
+      <c r="B32" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C32" s="1">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1">
+        <v>5</v>
+      </c>
+      <c r="E32" s="1">
+        <v>10</v>
+      </c>
+      <c r="F32" s="1">
+        <v>10</v>
+      </c>
       <c r="G32" s="1">
         <v>10</v>
       </c>
       <c r="H32" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I32" s="1">
+        <v>2</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
+      <c r="B33" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C33" s="1">
+        <v>3</v>
+      </c>
+      <c r="D33" s="1">
+        <v>5</v>
+      </c>
+      <c r="E33" s="1">
+        <v>10</v>
+      </c>
+      <c r="F33" s="1">
+        <v>10</v>
+      </c>
       <c r="G33" s="1">
         <v>10</v>
       </c>
       <c r="H33" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
+      <c r="B34" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C34" s="1">
+        <v>3</v>
+      </c>
+      <c r="D34" s="1">
+        <v>5</v>
+      </c>
+      <c r="E34" s="1">
+        <v>10</v>
+      </c>
+      <c r="F34" s="1">
+        <v>10</v>
+      </c>
       <c r="G34" s="1">
         <v>10</v>
       </c>
       <c r="H34" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
+      <c r="B35" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2</v>
+      </c>
+      <c r="D35" s="1">
+        <v>10</v>
+      </c>
+      <c r="E35" s="1">
+        <v>10</v>
+      </c>
+      <c r="F35" s="1">
+        <v>7</v>
+      </c>
       <c r="G35" s="1">
         <v>10</v>
       </c>
       <c r="H35" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.7</v>
+      </c>
+      <c r="I35" s="1">
+        <v>3</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1227,21 +1533,45 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J36" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
+      <c r="B37" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2</v>
+      </c>
+      <c r="D37" s="1">
+        <v>10</v>
+      </c>
+      <c r="E37" s="1">
+        <v>10</v>
+      </c>
+      <c r="F37" s="1">
+        <v>3</v>
+      </c>
       <c r="G37" s="1">
         <v>10</v>
       </c>
       <c r="H37" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.3</v>
+      </c>
+      <c r="I37" s="1">
+        <v>3</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1254,33 +1584,72 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
+      <c r="B39" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="C39" s="1">
+        <v>3</v>
+      </c>
+      <c r="D39" s="1">
+        <v>4</v>
+      </c>
+      <c r="E39" s="1">
+        <v>10</v>
+      </c>
+      <c r="F39" s="1">
+        <v>10</v>
+      </c>
       <c r="G39" s="1">
         <v>10</v>
       </c>
       <c r="H39" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I39" s="1">
+        <v>4</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
+      <c r="B40" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C40" s="1">
+        <v>3</v>
+      </c>
+      <c r="D40" s="1">
+        <v>5</v>
+      </c>
+      <c r="E40" s="1">
+        <v>10</v>
+      </c>
+      <c r="F40" s="1">
+        <v>10</v>
+      </c>
       <c r="G40" s="1">
         <v>10</v>
       </c>
       <c r="H40" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1293,7 +1662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1306,7 +1675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1319,7 +1688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1332,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1345,7 +1714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1358,7 +1727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1371,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <f t="shared" si="0"/>
         <v>46</v>

</xml_diff>

<commit_message>
Added evaluation for constellations until 72.
</commit_message>
<xml_diff>
--- a/thesis_data/evaluation_data/evaluation_data.xlsx
+++ b/thesis_data/evaluation_data/evaluation_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="26">
   <si>
     <t>constellation nb</t>
   </si>
@@ -72,7 +72,28 @@
     <t>GreLum</t>
   </si>
   <si>
-    <t>some cases GreLum, some LowDiff. Hard because of only 3 stars in constellation</t>
+    <t>maybe remove some stars from model for better accuracy</t>
+  </si>
+  <si>
+    <t>LowDiff</t>
+  </si>
+  <si>
+    <t>3 stars; very hard to detect</t>
+  </si>
+  <si>
+    <t>(?)some cases GreLum, some LowDiff</t>
+  </si>
+  <si>
+    <t>problems</t>
+  </si>
+  <si>
+    <t>raise AT for lower time</t>
+  </si>
+  <si>
+    <t>20 stars; very hard to detect</t>
+  </si>
+  <si>
+    <t>2 stars; impossible to detect</t>
   </si>
 </sst>
 </file>
@@ -417,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K91"/>
+  <dimension ref="A1:L91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,10 +451,11 @@
     <col min="7" max="8" width="13.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="17.85546875" style="1" customWidth="1"/>
     <col min="10" max="10" width="34.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="35.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,10 +487,13 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -500,11 +525,11 @@
       <c r="J2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>1</v>
@@ -516,11 +541,14 @@
         <f>F3/G3</f>
         <v>0</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A67" si="0">A3+1</f>
         <v>2</v>
@@ -551,7 +579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -582,7 +610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -616,7 +644,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -647,7 +675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -681,7 +709,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -712,7 +740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -746,7 +774,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -777,7 +805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -808,7 +836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -842,7 +870,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -854,8 +882,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -886,7 +917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -897,6 +928,9 @@
       <c r="H16" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1425,7 +1459,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1456,7 +1490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1487,7 +1521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1521,7 +1555,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1534,10 +1568,13 @@
         <v>0</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1571,7 +1608,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1583,8 +1620,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K38" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1618,7 +1658,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1649,332 +1689,821 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
+      <c r="B41" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C41" s="1">
+        <v>2</v>
+      </c>
+      <c r="D41" s="1">
+        <v>10</v>
+      </c>
+      <c r="E41" s="1">
+        <v>10</v>
+      </c>
+      <c r="F41" s="1">
+        <v>2</v>
+      </c>
       <c r="G41" s="1">
         <v>10</v>
       </c>
       <c r="H41" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+      <c r="I41" s="1">
+        <v>0</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
+      <c r="B42" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C42" s="1">
+        <v>3</v>
+      </c>
+      <c r="D42" s="1">
+        <v>2</v>
+      </c>
+      <c r="E42" s="1">
+        <v>5</v>
+      </c>
+      <c r="F42" s="1">
+        <v>10</v>
+      </c>
       <c r="G42" s="1">
         <v>10</v>
       </c>
       <c r="H42" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I42" s="1">
+        <v>5</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
+      <c r="B43" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C43" s="1">
+        <v>3</v>
+      </c>
+      <c r="D43" s="1">
+        <v>12</v>
+      </c>
+      <c r="E43" s="1">
+        <v>10</v>
+      </c>
+      <c r="F43" s="1">
+        <v>10</v>
+      </c>
       <c r="G43" s="1">
         <v>10</v>
       </c>
       <c r="H43" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I43" s="1">
+        <v>3</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
+      <c r="B44" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C44" s="1">
+        <v>5</v>
+      </c>
+      <c r="D44" s="1">
+        <v>3</v>
+      </c>
+      <c r="E44" s="1">
+        <v>20</v>
+      </c>
+      <c r="F44" s="1">
+        <v>6</v>
+      </c>
       <c r="G44" s="1">
         <v>10</v>
       </c>
       <c r="H44" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.6</v>
+      </c>
+      <c r="I44" s="1">
+        <v>0</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
+      <c r="B45" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="C45" s="1">
+        <v>3</v>
+      </c>
+      <c r="D45" s="1">
+        <v>5</v>
+      </c>
+      <c r="E45" s="1">
+        <v>10</v>
+      </c>
+      <c r="F45" s="1">
+        <v>10</v>
+      </c>
       <c r="G45" s="1">
         <v>10</v>
       </c>
       <c r="H45" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
+      <c r="B46" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C46" s="1">
+        <v>3</v>
+      </c>
+      <c r="D46" s="1">
+        <v>5</v>
+      </c>
+      <c r="E46" s="1">
+        <v>10</v>
+      </c>
+      <c r="F46" s="1">
+        <v>10</v>
+      </c>
       <c r="G46" s="1">
         <v>10</v>
       </c>
       <c r="H46" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
+      <c r="B47" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C47" s="1">
+        <v>3</v>
+      </c>
+      <c r="D47" s="1">
+        <v>12</v>
+      </c>
+      <c r="E47" s="1">
+        <v>10</v>
+      </c>
+      <c r="F47" s="1">
+        <v>9</v>
+      </c>
       <c r="G47" s="1">
         <v>10</v>
       </c>
       <c r="H47" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.9</v>
+      </c>
+      <c r="I47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
+      <c r="B48" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C48" s="1">
+        <v>3</v>
+      </c>
+      <c r="D48" s="1">
+        <v>5</v>
+      </c>
+      <c r="E48" s="1">
+        <v>10</v>
+      </c>
+      <c r="F48" s="1">
+        <v>10</v>
+      </c>
       <c r="G48" s="1">
         <v>10</v>
       </c>
       <c r="H48" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I48" s="1">
+        <v>2</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
+      <c r="B49" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C49" s="1">
+        <v>3</v>
+      </c>
+      <c r="D49" s="1">
+        <v>5</v>
+      </c>
+      <c r="E49" s="1">
+        <v>10</v>
+      </c>
+      <c r="F49" s="1">
+        <v>10</v>
+      </c>
       <c r="G49" s="1">
         <v>10</v>
       </c>
       <c r="H49" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
+      <c r="B50" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C50" s="1">
+        <v>2</v>
+      </c>
+      <c r="D50" s="1">
+        <v>5</v>
+      </c>
+      <c r="E50" s="1">
+        <v>10</v>
+      </c>
+      <c r="F50" s="1">
+        <v>6</v>
+      </c>
       <c r="G50" s="1">
         <v>10</v>
       </c>
       <c r="H50" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.6</v>
+      </c>
+      <c r="I50" s="1">
+        <v>2</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
+      <c r="B51" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C51" s="1">
+        <v>3</v>
+      </c>
+      <c r="D51" s="1">
+        <v>5</v>
+      </c>
+      <c r="E51" s="1">
+        <v>10</v>
+      </c>
+      <c r="F51" s="1">
+        <v>10</v>
+      </c>
       <c r="G51" s="1">
         <v>10</v>
       </c>
       <c r="H51" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
+      <c r="B52" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C52" s="1">
+        <v>2</v>
+      </c>
+      <c r="D52" s="1">
+        <v>10</v>
+      </c>
+      <c r="E52" s="1">
+        <v>5</v>
+      </c>
+      <c r="F52" s="1">
+        <v>10</v>
+      </c>
       <c r="G52" s="1">
         <v>10</v>
       </c>
       <c r="H52" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I52" s="1">
+        <v>7</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
+      <c r="B53" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C53" s="1">
+        <v>3</v>
+      </c>
+      <c r="D53" s="1">
+        <v>5</v>
+      </c>
+      <c r="E53" s="1">
+        <v>10</v>
+      </c>
+      <c r="F53" s="1">
+        <v>9</v>
+      </c>
       <c r="G53" s="1">
         <v>10</v>
       </c>
       <c r="H53" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.9</v>
+      </c>
+      <c r="I53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
+      <c r="B54" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C54" s="1">
+        <v>3</v>
+      </c>
+      <c r="D54" s="1">
+        <v>1</v>
+      </c>
+      <c r="E54" s="1">
+        <v>10</v>
+      </c>
+      <c r="F54" s="1">
+        <v>10</v>
+      </c>
       <c r="G54" s="1">
         <v>10</v>
       </c>
       <c r="H54" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I54" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
+      <c r="B55" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C55" s="1">
+        <v>5</v>
+      </c>
+      <c r="D55" s="1">
+        <v>5</v>
+      </c>
+      <c r="E55" s="1">
+        <v>10</v>
+      </c>
+      <c r="F55" s="1">
+        <v>7</v>
+      </c>
       <c r="G55" s="1">
         <v>10</v>
       </c>
       <c r="H55" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.7</v>
+      </c>
+      <c r="I55" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
+      <c r="B56" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C56" s="1">
+        <v>3</v>
+      </c>
+      <c r="D56" s="1">
+        <v>5</v>
+      </c>
+      <c r="E56" s="1">
+        <v>7</v>
+      </c>
+      <c r="F56" s="1">
+        <v>8</v>
+      </c>
       <c r="G56" s="1">
         <v>10</v>
       </c>
       <c r="H56" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.8</v>
+      </c>
+      <c r="I56" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
+      <c r="B57" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C57" s="1">
+        <v>3</v>
+      </c>
+      <c r="D57" s="1">
+        <v>3</v>
+      </c>
+      <c r="E57" s="1">
+        <v>10</v>
+      </c>
+      <c r="F57" s="1">
+        <v>10</v>
+      </c>
       <c r="G57" s="1">
         <v>10</v>
       </c>
       <c r="H57" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I57" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
+      <c r="B58" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="C58" s="1">
+        <v>3</v>
+      </c>
+      <c r="D58" s="1">
+        <v>3</v>
+      </c>
+      <c r="E58" s="1">
+        <v>10</v>
+      </c>
+      <c r="F58" s="1">
+        <v>10</v>
+      </c>
       <c r="G58" s="1">
         <v>10</v>
       </c>
       <c r="H58" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I58" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
+      <c r="B59" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="C59" s="1">
+        <v>5</v>
+      </c>
+      <c r="D59" s="1">
+        <v>3</v>
+      </c>
+      <c r="E59" s="1">
+        <v>10</v>
+      </c>
+      <c r="F59" s="1">
+        <v>7</v>
+      </c>
       <c r="G59" s="1">
         <v>10</v>
       </c>
       <c r="H59" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.7</v>
+      </c>
+      <c r="I59" s="1">
+        <v>2</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
+      <c r="B60" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C60" s="1">
+        <v>3</v>
+      </c>
+      <c r="D60" s="1">
+        <v>5</v>
+      </c>
+      <c r="E60" s="1">
+        <v>10</v>
+      </c>
+      <c r="F60" s="1">
+        <v>7</v>
+      </c>
       <c r="G60" s="1">
         <v>10</v>
       </c>
       <c r="H60" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.7</v>
+      </c>
+      <c r="I60" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
+      <c r="B61" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C61" s="1">
+        <v>5</v>
+      </c>
+      <c r="D61" s="1">
+        <v>5</v>
+      </c>
+      <c r="E61" s="1">
+        <v>40</v>
+      </c>
+      <c r="F61" s="1">
+        <v>7</v>
+      </c>
       <c r="G61" s="1">
         <v>10</v>
       </c>
       <c r="H61" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.7</v>
+      </c>
+      <c r="I61" s="1">
+        <v>6</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
+      <c r="B62" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C62" s="1">
+        <v>4</v>
+      </c>
+      <c r="D62" s="1">
+        <v>5</v>
+      </c>
+      <c r="E62" s="1">
+        <v>10</v>
+      </c>
+      <c r="F62" s="1">
+        <v>10</v>
+      </c>
       <c r="G62" s="1">
         <v>10</v>
       </c>
       <c r="H62" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I62" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
+      <c r="B63" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C63" s="1">
+        <v>3</v>
+      </c>
+      <c r="D63" s="1">
+        <v>5</v>
+      </c>
+      <c r="E63" s="1">
+        <v>10</v>
+      </c>
+      <c r="F63" s="1">
+        <v>10</v>
+      </c>
       <c r="G63" s="1">
         <v>10</v>
       </c>
       <c r="H63" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I63" s="1">
+        <v>1</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
+      <c r="B64" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C64" s="1">
+        <v>3</v>
+      </c>
+      <c r="D64" s="1">
+        <v>3</v>
+      </c>
+      <c r="E64" s="1">
+        <v>10</v>
+      </c>
+      <c r="F64" s="1">
+        <v>4</v>
+      </c>
       <c r="G64" s="1">
         <v>10</v>
       </c>
       <c r="H64" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.4</v>
+      </c>
+      <c r="I64" s="1">
+        <v>2</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
+      <c r="B65" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C65" s="1">
+        <v>3</v>
+      </c>
+      <c r="D65" s="1">
+        <v>5</v>
+      </c>
+      <c r="E65" s="1">
+        <v>10</v>
+      </c>
+      <c r="F65" s="1">
+        <v>10</v>
+      </c>
       <c r="G65" s="1">
         <v>10</v>
       </c>
       <c r="H65" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I65" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -1986,47 +2515,113 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K66" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
+      <c r="B67" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C67" s="1">
+        <v>3</v>
+      </c>
+      <c r="D67" s="1">
+        <v>10</v>
+      </c>
+      <c r="E67" s="1">
+        <v>10</v>
+      </c>
+      <c r="F67" s="1">
+        <v>6</v>
+      </c>
       <c r="G67" s="1">
         <v>10</v>
       </c>
       <c r="H67" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.6</v>
+      </c>
+      <c r="I67" s="1">
+        <v>1</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <f t="shared" ref="A68:A91" si="2">A67+1</f>
         <v>66</v>
       </c>
+      <c r="B68" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C68" s="1">
+        <v>3</v>
+      </c>
+      <c r="D68" s="1">
+        <v>10</v>
+      </c>
+      <c r="E68" s="1">
+        <v>10</v>
+      </c>
+      <c r="F68" s="1">
+        <v>9</v>
+      </c>
       <c r="G68" s="1">
         <v>10</v>
       </c>
       <c r="H68" s="1">
         <f t="shared" ref="H68:H91" si="3">F68/G68</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.9</v>
+      </c>
+      <c r="I68" s="1">
+        <v>5</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <f t="shared" si="2"/>
         <v>67</v>
       </c>
+      <c r="B69" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="C69" s="1">
+        <v>3</v>
+      </c>
+      <c r="D69" s="1">
+        <v>5</v>
+      </c>
+      <c r="E69" s="1">
+        <v>10</v>
+      </c>
+      <c r="F69" s="1">
+        <v>10</v>
+      </c>
       <c r="G69" s="1">
         <v>10</v>
       </c>
       <c r="H69" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I69" s="1">
+        <v>1</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <f t="shared" si="2"/>
         <v>68</v>
@@ -2038,60 +2633,138 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K70" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <f t="shared" si="2"/>
         <v>69</v>
       </c>
+      <c r="B71" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C71" s="1">
+        <v>3</v>
+      </c>
+      <c r="D71" s="1">
+        <v>3</v>
+      </c>
+      <c r="E71" s="1">
+        <v>10</v>
+      </c>
+      <c r="F71" s="1">
+        <v>10</v>
+      </c>
       <c r="G71" s="1">
         <v>10</v>
       </c>
       <c r="H71" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I71" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
+      <c r="B72" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C72" s="1">
+        <v>7</v>
+      </c>
+      <c r="D72" s="1">
+        <v>5</v>
+      </c>
+      <c r="E72" s="1">
+        <v>10</v>
+      </c>
+      <c r="F72" s="1">
+        <v>6</v>
+      </c>
       <c r="G72" s="1">
         <v>10</v>
       </c>
       <c r="H72" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.6</v>
+      </c>
+      <c r="I72" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <f t="shared" si="2"/>
         <v>71</v>
       </c>
+      <c r="B73" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C73" s="1">
+        <v>5</v>
+      </c>
+      <c r="D73" s="1">
+        <v>3</v>
+      </c>
+      <c r="E73" s="1">
+        <v>10</v>
+      </c>
+      <c r="F73" s="1">
+        <v>10</v>
+      </c>
       <c r="G73" s="1">
         <v>10</v>
       </c>
       <c r="H73" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I73" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <f t="shared" si="2"/>
         <v>72</v>
       </c>
+      <c r="B74" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C74" s="1">
+        <v>3</v>
+      </c>
+      <c r="D74" s="1">
+        <v>3</v>
+      </c>
+      <c r="E74" s="1">
+        <v>10</v>
+      </c>
+      <c r="F74" s="1">
+        <v>10</v>
+      </c>
       <c r="G74" s="1">
         <v>10</v>
       </c>
       <c r="H74" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I74" s="1">
+        <v>1</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <f t="shared" si="2"/>
         <v>73</v>
@@ -2104,7 +2777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <f t="shared" si="2"/>
         <v>74</v>
@@ -2117,7 +2790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <f t="shared" si="2"/>
         <v>75</v>
@@ -2130,7 +2803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <f t="shared" si="2"/>
         <v>76</v>
@@ -2143,7 +2816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <f t="shared" si="2"/>
         <v>77</v>
@@ -2156,7 +2829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <f t="shared" si="2"/>
         <v>78</v>

</xml_diff>

<commit_message>
Refactoring. Added custom parameters for each constellation.
</commit_message>
<xml_diff>
--- a/thesis_data/evaluation_data/evaluation_data.xlsx
+++ b/thesis_data/evaluation_data/evaluation_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="32">
   <si>
     <t>constellation nb</t>
   </si>
@@ -459,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="J13" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,7 +1124,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1162,7 +1162,7 @@
         <v>15,0.05,2,5,10,2</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1203,7 +1203,7 @@
         <v>16,0.1,3,10,10,2</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1241,7 +1241,7 @@
         <v>17,0.02,2,7,10,2</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -1279,7 +1279,7 @@
         <v>18,0.1,3,7,10,2</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1320,7 +1320,7 @@
         <v>19,0.1,3,10,10,0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1361,7 +1361,7 @@
         <v>20,0.1,1,10,7,0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1402,7 +1402,7 @@
         <v>21,0.1,3,5,10,2</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1443,7 +1443,7 @@
         <v>22,0.01,3,3,10,2</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1484,7 +1484,7 @@
         <v>23,0.05,3,5,10,2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -1518,14 +1518,17 @@
         <v>14</v>
       </c>
       <c r="K26" s="1">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" si="0"/>
-        <v>24,0.05,3,3,10,2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>24,0.05,3,3,10,-1</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -1566,7 +1569,7 @@
         <v>25,0.5,3,5,20,2</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -1604,7 +1607,7 @@
         <v>26,0.05,3,3,10,2</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -1642,7 +1645,7 @@
         <v>27,0.05,3,3,10,2</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -1680,7 +1683,7 @@
         <v>28,0.05,3,3,10,2</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -1721,7 +1724,7 @@
         <v>29,0.05,3,3,10,0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="1"/>
         <v>30</v>

</xml_diff>

<commit_message>
Added drawing of lines and name of constellation detected for constellations up until 75.
</commit_message>
<xml_diff>
--- a/thesis_data/evaluation_data/evaluation_data.xlsx
+++ b/thesis_data/evaluation_data/evaluation_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="112">
   <si>
     <t>file name</t>
   </si>
@@ -346,6 +346,12 @@
   </si>
   <si>
     <t>Total Time Of Detection</t>
+  </si>
+  <si>
+    <t>other constellations detected(without degenerate triangles)</t>
+  </si>
+  <si>
+    <t>time(seconds) w/ parallelization without degenerate triangles</t>
   </si>
 </sst>
 </file>
@@ -699,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H113"/>
+  <dimension ref="A1:J113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C85" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" topLeftCell="D19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,7 +720,7 @@
     <col min="6" max="13" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -728,13 +734,19 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
@@ -747,14 +759,14 @@
       <c r="F2" s="1">
         <v>0</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>342</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
@@ -767,14 +779,14 @@
       <c r="F3" s="1">
         <v>11</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>197</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
@@ -787,14 +799,14 @@
       <c r="F4" s="1">
         <v>6</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>303</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
@@ -807,11 +819,11 @@
       <c r="F5" s="1">
         <v>8</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>640</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
@@ -824,11 +836,11 @@
       <c r="F6" s="1">
         <v>5</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>1417</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
@@ -841,11 +853,11 @@
       <c r="F7" s="1">
         <v>5</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>902</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
@@ -858,14 +870,14 @@
       <c r="F8" s="1">
         <v>0</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>61</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
@@ -878,14 +890,14 @@
       <c r="F9" s="1">
         <v>0</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <v>118</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
@@ -898,14 +910,14 @@
       <c r="F10" s="1">
         <v>2</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <v>212</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
@@ -918,14 +930,14 @@
       <c r="F11" s="1">
         <v>0</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
         <v>76</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>15</v>
       </c>
@@ -938,14 +950,14 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <v>94</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -964,14 +976,14 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <v>58</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>51</v>
       </c>
@@ -990,12 +1002,12 @@
       <c r="F14" s="1">
         <v>0</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1">
+      <c r="H14" s="1"/>
+      <c r="I14" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>33</v>
       </c>
@@ -1014,12 +1026,12 @@
       <c r="F15" s="1">
         <v>0</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1">
+      <c r="H15" s="1"/>
+      <c r="I15" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>59</v>
       </c>
@@ -1038,12 +1050,12 @@
       <c r="F16" s="1">
         <v>4</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1">
+      <c r="H16" s="1"/>
+      <c r="I16" s="1">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>26</v>
       </c>
@@ -1062,11 +1074,11 @@
       <c r="F17" s="1">
         <v>0</v>
       </c>
-      <c r="H17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>67</v>
       </c>
@@ -1085,11 +1097,14 @@
       <c r="F18" s="1">
         <v>5</v>
       </c>
-      <c r="H18" s="1">
+      <c r="G18" s="1">
+        <v>5</v>
+      </c>
+      <c r="I18" s="1">
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>87</v>
       </c>
@@ -1108,11 +1123,11 @@
       <c r="F19" s="1">
         <v>1</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I19" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>3</v>
       </c>
@@ -1131,11 +1146,11 @@
       <c r="F20" s="1">
         <v>0</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1154,11 +1169,11 @@
       <c r="F21" s="1">
         <v>0</v>
       </c>
-      <c r="H21" s="1">
+      <c r="I21" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>22</v>
       </c>
@@ -1177,11 +1192,11 @@
       <c r="F22" s="1">
         <v>0</v>
       </c>
-      <c r="H22" s="1">
+      <c r="I22" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>9</v>
       </c>
@@ -1200,11 +1215,11 @@
       <c r="F23" s="1">
         <v>0</v>
       </c>
-      <c r="H23" s="1">
+      <c r="I23" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>38</v>
       </c>
@@ -1223,11 +1238,11 @@
       <c r="F24" s="1">
         <v>1</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>51</v>
       </c>
@@ -1246,11 +1261,11 @@
       <c r="F25" s="1">
         <v>0</v>
       </c>
-      <c r="H25" s="1">
+      <c r="I25" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>86</v>
       </c>
@@ -1269,11 +1284,11 @@
       <c r="F26" s="1">
         <v>1</v>
       </c>
-      <c r="H26" s="1">
+      <c r="I26" s="1">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>75</v>
       </c>
@@ -1292,11 +1307,11 @@
       <c r="F27" s="1">
         <v>0</v>
       </c>
-      <c r="H27" s="1">
+      <c r="I27" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>11</v>
       </c>
@@ -1315,11 +1330,11 @@
       <c r="F28" s="1">
         <v>2</v>
       </c>
-      <c r="H28" s="1">
+      <c r="I28" s="1">
         <v>365</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>51</v>
       </c>
@@ -1338,11 +1353,11 @@
       <c r="F29" s="1">
         <v>1</v>
       </c>
-      <c r="H29" s="1">
+      <c r="I29" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>4</v>
       </c>
@@ -1361,11 +1376,11 @@
       <c r="F30" s="1">
         <v>0</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>72</v>
       </c>
@@ -1384,11 +1399,11 @@
       <c r="F31" s="1">
         <v>0</v>
       </c>
-      <c r="H31" s="1">
+      <c r="I31" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>60</v>
       </c>
@@ -1407,11 +1422,11 @@
       <c r="F32" s="1">
         <v>5</v>
       </c>
-      <c r="H32" s="1">
+      <c r="I32" s="1">
         <v>241</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>52</v>
       </c>
@@ -1430,11 +1445,11 @@
       <c r="F33" s="1">
         <v>0</v>
       </c>
-      <c r="H33" s="1">
+      <c r="I33" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>23</v>
       </c>
@@ -1453,11 +1468,11 @@
       <c r="F34" s="1">
         <v>4</v>
       </c>
-      <c r="H34" s="1">
+      <c r="I34" s="1">
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>54</v>
       </c>
@@ -1476,11 +1491,11 @@
       <c r="F35" s="1">
         <v>0</v>
       </c>
-      <c r="H35" s="1">
+      <c r="I35" s="1">
         <v>216</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>49</v>
       </c>
@@ -1499,11 +1514,11 @@
       <c r="F36" s="1">
         <v>0</v>
       </c>
-      <c r="H36" s="1">
+      <c r="I36" s="1">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>44</v>
       </c>
@@ -1522,11 +1537,11 @@
       <c r="F37" s="1">
         <v>0</v>
       </c>
-      <c r="H37" s="1">
+      <c r="I37" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>62</v>
       </c>
@@ -1545,11 +1560,11 @@
       <c r="F38" s="1">
         <v>13</v>
       </c>
-      <c r="H38" s="1">
+      <c r="I38" s="1">
         <v>758</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>29</v>
       </c>
@@ -1568,11 +1583,11 @@
       <c r="F39" s="1">
         <v>1</v>
       </c>
-      <c r="H39" s="1">
+      <c r="I39" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>55</v>
       </c>
@@ -1591,11 +1606,11 @@
       <c r="F40" s="1">
         <v>9</v>
       </c>
-      <c r="H40" s="1">
+      <c r="I40" s="1">
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>13</v>
       </c>
@@ -1614,11 +1629,11 @@
       <c r="F41" s="1">
         <v>1</v>
       </c>
-      <c r="H41" s="1">
+      <c r="I41" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>15</v>
       </c>
@@ -1637,11 +1652,11 @@
       <c r="F42" s="1">
         <v>1</v>
       </c>
-      <c r="H42" s="1">
+      <c r="I42" s="1">
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>26</v>
       </c>
@@ -1660,11 +1675,11 @@
       <c r="F43" s="1">
         <v>0</v>
       </c>
-      <c r="H43" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>49</v>
       </c>
@@ -1683,11 +1698,11 @@
       <c r="F44" s="1">
         <v>2</v>
       </c>
-      <c r="H44" s="1">
+      <c r="I44" s="1">
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>4</v>
       </c>
@@ -1706,11 +1721,11 @@
       <c r="F45" s="1">
         <v>0</v>
       </c>
-      <c r="H45" s="1">
+      <c r="I45" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>59</v>
       </c>
@@ -1729,11 +1744,11 @@
       <c r="F46" s="1">
         <v>2</v>
       </c>
-      <c r="H46" s="1">
+      <c r="I46" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>52</v>
       </c>
@@ -1752,11 +1767,11 @@
       <c r="F47" s="1">
         <v>0</v>
       </c>
-      <c r="H47" s="1">
+      <c r="I47" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>78</v>
       </c>
@@ -1775,11 +1790,15 @@
       <c r="F48" s="1">
         <v>18</v>
       </c>
-      <c r="H48" s="1">
+      <c r="G48" s="1">
+        <v>13</v>
+      </c>
+      <c r="I48" s="1">
         <v>390</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>47</v>
       </c>
@@ -1798,11 +1817,11 @@
       <c r="F49" s="1">
         <v>0</v>
       </c>
-      <c r="H49" s="1">
+      <c r="I49" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>25</v>
       </c>
@@ -1821,11 +1840,11 @@
       <c r="F50" s="1">
         <v>0</v>
       </c>
-      <c r="H50" s="1">
+      <c r="I50" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>72</v>
       </c>
@@ -1844,11 +1863,17 @@
       <c r="F51" s="1">
         <v>11</v>
       </c>
-      <c r="H51" s="1">
+      <c r="G51" s="1">
+        <v>8</v>
+      </c>
+      <c r="I51" s="1">
         <v>355</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J51" s="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>50</v>
       </c>
@@ -1867,11 +1892,11 @@
       <c r="F52" s="1">
         <v>0</v>
       </c>
-      <c r="H52" s="1">
+      <c r="I52" s="1">
         <v>31</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>17</v>
       </c>
@@ -1890,11 +1915,11 @@
       <c r="F53" s="1">
         <v>1</v>
       </c>
-      <c r="H53" s="1">
+      <c r="I53" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>44</v>
       </c>
@@ -1913,11 +1938,11 @@
       <c r="F54" s="1">
         <v>0</v>
       </c>
-      <c r="H54" s="1">
+      <c r="I54" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>32</v>
       </c>
@@ -1936,11 +1961,11 @@
       <c r="F55" s="1">
         <v>0</v>
       </c>
-      <c r="H55" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>5</v>
       </c>
@@ -1959,11 +1984,11 @@
       <c r="F56" s="1">
         <v>1</v>
       </c>
-      <c r="H56" s="1">
+      <c r="I56" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>60</v>
       </c>
@@ -1982,11 +2007,11 @@
       <c r="F57" s="1">
         <v>2</v>
       </c>
-      <c r="H57" s="1">
+      <c r="I57" s="1">
         <v>231</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>11</v>
       </c>
@@ -2005,11 +2030,11 @@
       <c r="F58" s="1">
         <v>0</v>
       </c>
-      <c r="H58" s="1">
+      <c r="I58" s="1">
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>50</v>
       </c>
@@ -2028,11 +2053,11 @@
       <c r="F59" s="1">
         <v>0</v>
       </c>
-      <c r="H59" s="1">
+      <c r="I59" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>70</v>
       </c>
@@ -2051,11 +2076,11 @@
       <c r="F60" s="1">
         <v>6</v>
       </c>
-      <c r="H60" s="1">
+      <c r="I60" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>4</v>
       </c>
@@ -2074,11 +2099,11 @@
       <c r="F61" s="1">
         <v>0</v>
       </c>
-      <c r="H61" s="1">
+      <c r="I61" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>5</v>
       </c>
@@ -2097,11 +2122,11 @@
       <c r="F62" s="1">
         <v>0</v>
       </c>
-      <c r="H62" s="1">
+      <c r="I62" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>20</v>
       </c>
@@ -2120,11 +2145,11 @@
       <c r="F63" s="1">
         <v>0</v>
       </c>
-      <c r="H63" s="1">
+      <c r="I63" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>31</v>
       </c>
@@ -2143,11 +2168,11 @@
       <c r="F64" s="1">
         <v>0</v>
       </c>
-      <c r="H64" s="1">
+      <c r="I64" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>53</v>
       </c>
@@ -2166,11 +2191,11 @@
       <c r="F65" s="1">
         <v>0</v>
       </c>
-      <c r="H65" s="1">
+      <c r="I65" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>30</v>
       </c>
@@ -2189,11 +2214,11 @@
       <c r="F66" s="1">
         <v>0</v>
       </c>
-      <c r="H66" s="1">
+      <c r="I66" s="1">
         <v>123</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -2212,11 +2237,11 @@
       <c r="F67" s="1">
         <v>0</v>
       </c>
-      <c r="H67" s="1">
+      <c r="I67" s="1">
         <v>430</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>60</v>
       </c>
@@ -2235,11 +2260,11 @@
       <c r="F68" s="1">
         <v>1</v>
       </c>
-      <c r="H68" s="1">
+      <c r="I68" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>65</v>
       </c>
@@ -2258,11 +2283,11 @@
       <c r="F69" s="1">
         <v>0</v>
       </c>
-      <c r="H69" s="1">
+      <c r="I69" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>9</v>
       </c>
@@ -2281,11 +2306,11 @@
       <c r="F70" s="1">
         <v>0</v>
       </c>
-      <c r="H70" s="1">
+      <c r="I70" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>82</v>
       </c>
@@ -2304,11 +2329,11 @@
       <c r="F71" s="1">
         <v>4</v>
       </c>
-      <c r="H71" s="1">
+      <c r="I71" s="1">
         <v>238</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>58</v>
       </c>
@@ -2327,11 +2352,11 @@
       <c r="F72" s="1">
         <v>3</v>
       </c>
-      <c r="H72" s="1">
+      <c r="I72" s="1">
         <v>165</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>8</v>
       </c>
@@ -2350,11 +2375,11 @@
       <c r="F73" s="1">
         <v>0</v>
       </c>
-      <c r="H73" s="1">
+      <c r="I73" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>31</v>
       </c>
@@ -2373,11 +2398,11 @@
       <c r="F74" s="1">
         <v>0</v>
       </c>
-      <c r="H74" s="1">
+      <c r="I74" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>30</v>
       </c>
@@ -2396,11 +2421,11 @@
       <c r="F75" s="1">
         <v>0</v>
       </c>
-      <c r="H75" s="1">
+      <c r="I75" s="1">
         <v>57</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>43</v>
       </c>
@@ -2419,11 +2444,11 @@
       <c r="F76" s="1">
         <v>0</v>
       </c>
-      <c r="H76" s="1">
+      <c r="I76" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>45</v>
       </c>
@@ -2442,11 +2467,11 @@
       <c r="F77" s="1">
         <v>0</v>
       </c>
-      <c r="H77" s="1">
+      <c r="I77" s="1">
         <v>31</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>19</v>
       </c>
@@ -2465,11 +2490,11 @@
       <c r="F78" s="1">
         <v>1</v>
       </c>
-      <c r="H78" s="1">
+      <c r="I78" s="1">
         <v>160</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>27</v>
       </c>
@@ -2488,11 +2513,11 @@
       <c r="F79" s="1">
         <v>0</v>
       </c>
-      <c r="H79" s="1">
+      <c r="I79" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>54</v>
       </c>
@@ -2511,11 +2536,11 @@
       <c r="F80" s="1">
         <v>0</v>
       </c>
-      <c r="H80" s="1">
+      <c r="I80" s="1">
         <v>81</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>11</v>
       </c>
@@ -2534,11 +2559,11 @@
       <c r="F81" s="1">
         <v>0</v>
       </c>
-      <c r="H81" s="1">
+      <c r="I81" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>76</v>
       </c>
@@ -2557,11 +2582,11 @@
       <c r="F82" s="1">
         <v>1</v>
       </c>
-      <c r="H82" s="1">
+      <c r="I82" s="1">
         <v>51</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>70</v>
       </c>
@@ -2580,11 +2605,11 @@
       <c r="F83" s="1">
         <v>0</v>
       </c>
-      <c r="H83" s="1">
+      <c r="I83" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>38</v>
       </c>
@@ -2603,11 +2628,11 @@
       <c r="F84" s="1">
         <v>1</v>
       </c>
-      <c r="H84" s="1">
+      <c r="I84" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>74</v>
       </c>
@@ -2626,11 +2651,11 @@
       <c r="F85" s="1">
         <v>1</v>
       </c>
-      <c r="H85" s="1">
+      <c r="I85" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>0</v>
       </c>
@@ -2649,11 +2674,11 @@
       <c r="F86" s="1">
         <v>0</v>
       </c>
-      <c r="H86" s="1">
+      <c r="I86" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -2672,11 +2697,11 @@
       <c r="F87" s="1">
         <v>3</v>
       </c>
-      <c r="H87" s="1">
+      <c r="I87" s="1">
         <v>614</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>58</v>
       </c>
@@ -2695,11 +2720,11 @@
       <c r="F88" s="1">
         <v>0</v>
       </c>
-      <c r="H88" s="1">
+      <c r="I88" s="1">
         <v>55</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>19</v>
       </c>
@@ -2718,11 +2743,11 @@
       <c r="F89" s="1">
         <v>1</v>
       </c>
-      <c r="H89" s="1">
+      <c r="I89" s="1">
         <v>156</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>60</v>
       </c>
@@ -2741,11 +2766,11 @@
       <c r="F90" s="1">
         <v>2</v>
       </c>
-      <c r="H90" s="1">
+      <c r="I90" s="1">
         <v>105</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>59</v>
       </c>
@@ -2764,11 +2789,11 @@
       <c r="F91" s="1">
         <v>0</v>
       </c>
-      <c r="H91" s="1">
+      <c r="I91" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>3</v>
       </c>
@@ -2787,11 +2812,11 @@
       <c r="F92" s="1">
         <v>0</v>
       </c>
-      <c r="H92" s="1">
+      <c r="I92" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>65</v>
       </c>
@@ -2810,11 +2835,11 @@
       <c r="F93" s="1">
         <v>0</v>
       </c>
-      <c r="H93" s="1">
+      <c r="I93" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>10</v>
       </c>
@@ -2833,11 +2858,11 @@
       <c r="F94" s="1">
         <v>0</v>
       </c>
-      <c r="H94" s="1">
+      <c r="I94" s="1">
         <v>38</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>30</v>
       </c>
@@ -2856,11 +2881,11 @@
       <c r="F95" s="1">
         <v>0</v>
       </c>
-      <c r="H95" s="1">
+      <c r="I95" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>60</v>
       </c>
@@ -2879,11 +2904,11 @@
       <c r="F96" s="1">
         <v>0</v>
       </c>
-      <c r="H96" s="1">
+      <c r="I96" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>77</v>
       </c>
@@ -2902,11 +2927,11 @@
       <c r="F97" s="1">
         <v>0</v>
       </c>
-      <c r="H97" s="1">
+      <c r="I97" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>72</v>
       </c>
@@ -2925,11 +2950,11 @@
       <c r="F98" s="1">
         <v>0</v>
       </c>
-      <c r="H98" s="1">
+      <c r="I98" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>65</v>
       </c>
@@ -2948,11 +2973,11 @@
       <c r="F99" s="1">
         <v>1</v>
       </c>
-      <c r="H99" s="1">
+      <c r="I99" s="1">
         <v>56</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>3</v>
       </c>
@@ -2971,11 +2996,11 @@
       <c r="F100" s="1">
         <v>0</v>
       </c>
-      <c r="H100" s="1">
+      <c r="I100" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>4</v>
       </c>
@@ -2994,11 +3019,11 @@
       <c r="F101" s="1">
         <v>1</v>
       </c>
-      <c r="H101" s="1">
+      <c r="I101" s="1">
         <v>69</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>25</v>
       </c>
@@ -3017,14 +3042,14 @@
       <c r="F102" s="1">
         <v>0</v>
       </c>
-      <c r="H102" s="1">
+      <c r="I102" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="C104" s="1" t="s">
         <v>105</v>
@@ -3038,11 +3063,11 @@
       <c r="F104" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="H104" s="1" t="s">
+      <c r="I104" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="C105" s="1">
         <f>ROWS(C8:C102)</f>
@@ -3060,30 +3085,30 @@
         <f>SUM(F8:F102)</f>
         <v>116</v>
       </c>
-      <c r="H105">
-        <f>SUM(H8:H102)</f>
+      <c r="I105">
+        <f>SUM(I8:I102)</f>
         <v>6751</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added drawing of lines and name of constellation detected for all constellations.
</commit_message>
<xml_diff>
--- a/thesis_data/evaluation_data/evaluation_data.xlsx
+++ b/thesis_data/evaluation_data/evaluation_data.xlsx
@@ -707,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,11 +870,17 @@
       <c r="F8" s="1">
         <v>0</v>
       </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
       <c r="H8" s="1">
         <v>61</v>
       </c>
       <c r="I8" s="1">
         <v>20</v>
+      </c>
+      <c r="J8" s="1">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -890,11 +896,17 @@
       <c r="F9" s="1">
         <v>0</v>
       </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
       <c r="H9" s="1">
         <v>118</v>
       </c>
       <c r="I9" s="1">
         <v>40</v>
+      </c>
+      <c r="J9" s="1">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -910,11 +922,17 @@
       <c r="F10" s="1">
         <v>2</v>
       </c>
+      <c r="G10" s="1">
+        <v>2</v>
+      </c>
       <c r="H10" s="1">
         <v>212</v>
       </c>
       <c r="I10" s="1">
         <v>67</v>
+      </c>
+      <c r="J10" s="1">
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -930,11 +948,17 @@
       <c r="F11" s="1">
         <v>0</v>
       </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
       <c r="H11" s="1">
         <v>76</v>
       </c>
       <c r="I11" s="1">
         <v>19</v>
+      </c>
+      <c r="J11" s="1">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -950,11 +974,17 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
       <c r="H12" s="1">
         <v>94</v>
       </c>
       <c r="I12" s="1">
         <v>45</v>
+      </c>
+      <c r="J12" s="1">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -976,11 +1006,17 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
       <c r="H13" s="1">
         <v>58</v>
       </c>
       <c r="I13" s="1">
         <v>24</v>
+      </c>
+      <c r="J13" s="1">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Filtered degenerate constellation triangles. Reevaluation for all images.
</commit_message>
<xml_diff>
--- a/thesis_data/evaluation_data/evaluation_data.xlsx
+++ b/thesis_data/evaluation_data/evaluation_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22035" windowHeight="9285"/>
+    <workbookView xWindow="285" yWindow="60" windowWidth="22035" windowHeight="9285"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="117">
   <si>
     <t>file name</t>
   </si>
@@ -348,10 +348,25 @@
     <t>Total Time Of Detection</t>
   </si>
   <si>
-    <t>other constellations detected(without degenerate triangles)</t>
-  </si>
-  <si>
     <t>time(seconds) w/ parallelization without degenerate triangles</t>
+  </si>
+  <si>
+    <t>other const det.(w/out degen. triangles)</t>
+  </si>
+  <si>
+    <t>Total False Constellations Detected(w/ degen. Filter)</t>
+  </si>
+  <si>
+    <t>Total Time Of Detection(w/ degen. Filter)</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>False Det. / Image</t>
+  </si>
+  <si>
+    <t>Time/Image</t>
   </si>
 </sst>
 </file>
@@ -705,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J113"/>
+  <dimension ref="A1:K113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="C97" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F109" sqref="F109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,10 +732,11 @@
     <col min="3" max="3" width="45.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="35.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="39.42578125" style="1" customWidth="1"/>
-    <col min="6" max="13" width="35.7109375" customWidth="1"/>
+    <col min="6" max="9" width="35.7109375" customWidth="1"/>
+    <col min="11" max="13" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -734,19 +750,19 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
@@ -759,14 +775,14 @@
       <c r="F2" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="1">
-        <v>342</v>
-      </c>
       <c r="I2" s="1">
         <v>141</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="1">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
@@ -779,14 +795,14 @@
       <c r="F3" s="1">
         <v>11</v>
       </c>
-      <c r="H3" s="1">
-        <v>197</v>
-      </c>
       <c r="I3" s="1">
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="1">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
@@ -799,14 +815,14 @@
       <c r="F4" s="1">
         <v>6</v>
       </c>
-      <c r="H4" s="1">
-        <v>303</v>
-      </c>
       <c r="I4" s="1">
         <v>116</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="1">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
@@ -819,11 +835,11 @@
       <c r="F5" s="1">
         <v>8</v>
       </c>
-      <c r="H5" s="1">
+      <c r="K5" s="1">
         <v>640</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
@@ -836,11 +852,11 @@
       <c r="F6" s="1">
         <v>5</v>
       </c>
-      <c r="H6" s="1">
+      <c r="K6" s="1">
         <v>1417</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
@@ -853,11 +869,11 @@
       <c r="F7" s="1">
         <v>5</v>
       </c>
-      <c r="H7" s="1">
+      <c r="K7" s="1">
         <v>902</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
@@ -874,16 +890,16 @@
         <v>0</v>
       </c>
       <c r="H8" s="1">
-        <v>61</v>
+        <v>14.59</v>
       </c>
       <c r="I8" s="1">
         <v>20</v>
       </c>
-      <c r="J8" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
@@ -900,16 +916,16 @@
         <v>0</v>
       </c>
       <c r="H9" s="1">
-        <v>118</v>
+        <v>25.5</v>
       </c>
       <c r="I9" s="1">
         <v>40</v>
       </c>
-      <c r="J9" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="1">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
@@ -923,19 +939,19 @@
         <v>2</v>
       </c>
       <c r="G10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10" s="1">
-        <v>212</v>
+        <v>41.9</v>
       </c>
       <c r="I10" s="1">
         <v>67</v>
       </c>
-      <c r="J10" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="1">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
@@ -952,16 +968,16 @@
         <v>0</v>
       </c>
       <c r="H11" s="1">
-        <v>76</v>
+        <v>13.84</v>
       </c>
       <c r="I11" s="1">
         <v>19</v>
       </c>
-      <c r="J11" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>15</v>
       </c>
@@ -975,19 +991,19 @@
         <v>1</v>
       </c>
       <c r="G12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="1">
-        <v>94</v>
+        <v>26.14</v>
       </c>
       <c r="I12" s="1">
         <v>45</v>
       </c>
-      <c r="J12" s="1">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -1010,16 +1026,16 @@
         <v>0</v>
       </c>
       <c r="H13" s="1">
-        <v>58</v>
+        <v>12.72</v>
       </c>
       <c r="I13" s="1">
         <v>24</v>
       </c>
-      <c r="J13" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>51</v>
       </c>
@@ -1038,12 +1054,18 @@
       <c r="F14" s="1">
         <v>0</v>
       </c>
-      <c r="H14" s="1"/>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>2.37</v>
+      </c>
       <c r="I14" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>33</v>
       </c>
@@ -1062,12 +1084,18 @@
       <c r="F15" s="1">
         <v>0</v>
       </c>
-      <c r="H15" s="1"/>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>11.1</v>
+      </c>
       <c r="I15" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>59</v>
       </c>
@@ -1086,10 +1114,16 @@
       <c r="F16" s="1">
         <v>4</v>
       </c>
-      <c r="H16" s="1"/>
+      <c r="G16" s="1">
+        <v>2</v>
+      </c>
+      <c r="H16" s="1">
+        <v>34.659999999999997</v>
+      </c>
       <c r="I16" s="1">
         <v>47</v>
       </c>
+      <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
@@ -1110,6 +1144,12 @@
       <c r="F17" s="1">
         <v>0</v>
       </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.96</v>
+      </c>
       <c r="I17" s="1">
         <v>1</v>
       </c>
@@ -1134,7 +1174,10 @@
         <v>5</v>
       </c>
       <c r="G18" s="1">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="H18" s="1">
+        <v>40.9</v>
       </c>
       <c r="I18" s="1">
         <v>61</v>
@@ -1159,6 +1202,12 @@
       <c r="F19" s="1">
         <v>1</v>
       </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1">
+        <v>4.8899999999999997</v>
+      </c>
       <c r="I19" s="1">
         <v>6</v>
       </c>
@@ -1182,6 +1231,12 @@
       <c r="F20" s="1">
         <v>0</v>
       </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>15.14</v>
+      </c>
       <c r="I20" s="1">
         <v>20</v>
       </c>
@@ -1205,6 +1260,12 @@
       <c r="F21" s="1">
         <v>0</v>
       </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>51.44</v>
+      </c>
       <c r="I21" s="1">
         <v>70</v>
       </c>
@@ -1228,6 +1289,12 @@
       <c r="F22" s="1">
         <v>0</v>
       </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>5.01</v>
+      </c>
       <c r="I22" s="1">
         <v>8</v>
       </c>
@@ -1251,6 +1318,12 @@
       <c r="F23" s="1">
         <v>0</v>
       </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1.5</v>
+      </c>
       <c r="I23" s="1">
         <v>2</v>
       </c>
@@ -1274,6 +1347,12 @@
       <c r="F24" s="1">
         <v>1</v>
       </c>
+      <c r="G24" s="1">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <v>19.75</v>
+      </c>
       <c r="I24" s="1">
         <v>31</v>
       </c>
@@ -1297,6 +1376,12 @@
       <c r="F25" s="1">
         <v>0</v>
       </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <v>16.57</v>
+      </c>
       <c r="I25" s="1">
         <v>25</v>
       </c>
@@ -1320,6 +1405,12 @@
       <c r="F26" s="1">
         <v>1</v>
       </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>37.71</v>
+      </c>
       <c r="I26" s="1">
         <v>51</v>
       </c>
@@ -1343,6 +1434,12 @@
       <c r="F27" s="1">
         <v>0</v>
       </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <v>16.77</v>
+      </c>
       <c r="I27" s="1">
         <v>24</v>
       </c>
@@ -1366,6 +1463,12 @@
       <c r="F28" s="1">
         <v>2</v>
       </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1">
+        <v>256.81</v>
+      </c>
       <c r="I28" s="1">
         <v>365</v>
       </c>
@@ -1389,6 +1492,12 @@
       <c r="F29" s="1">
         <v>1</v>
       </c>
+      <c r="G29" s="1">
+        <v>1</v>
+      </c>
+      <c r="H29" s="1">
+        <v>8.56</v>
+      </c>
       <c r="I29" s="1">
         <v>13</v>
       </c>
@@ -1412,6 +1521,12 @@
       <c r="F30" s="1">
         <v>0</v>
       </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
+        <v>10.24</v>
+      </c>
       <c r="I30" s="1">
         <v>15</v>
       </c>
@@ -1435,6 +1550,12 @@
       <c r="F31" s="1">
         <v>0</v>
       </c>
+      <c r="G31" s="1">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1">
+        <v>8.6</v>
+      </c>
       <c r="I31" s="1">
         <v>12</v>
       </c>
@@ -1458,11 +1579,17 @@
       <c r="F32" s="1">
         <v>5</v>
       </c>
+      <c r="G32" s="1">
+        <v>3</v>
+      </c>
+      <c r="H32" s="1">
+        <v>164.29</v>
+      </c>
       <c r="I32" s="1">
         <v>241</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>52</v>
       </c>
@@ -1481,11 +1608,17 @@
       <c r="F33" s="1">
         <v>0</v>
       </c>
+      <c r="G33" s="1">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1">
+        <v>10.87</v>
+      </c>
       <c r="I33" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>23</v>
       </c>
@@ -1504,11 +1637,17 @@
       <c r="F34" s="1">
         <v>4</v>
       </c>
+      <c r="G34" s="1">
+        <v>2</v>
+      </c>
+      <c r="H34" s="1">
+        <v>65.61</v>
+      </c>
       <c r="I34" s="1">
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>54</v>
       </c>
@@ -1527,11 +1666,17 @@
       <c r="F35" s="1">
         <v>0</v>
       </c>
+      <c r="G35" s="1">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1">
+        <v>162.4</v>
+      </c>
       <c r="I35" s="1">
         <v>216</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>49</v>
       </c>
@@ -1550,11 +1695,17 @@
       <c r="F36" s="1">
         <v>0</v>
       </c>
+      <c r="G36" s="1">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1">
+        <v>26.26</v>
+      </c>
       <c r="I36" s="1">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>44</v>
       </c>
@@ -1573,11 +1724,17 @@
       <c r="F37" s="1">
         <v>0</v>
       </c>
+      <c r="G37" s="1">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1">
+        <v>14</v>
+      </c>
       <c r="I37" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>62</v>
       </c>
@@ -1596,11 +1753,17 @@
       <c r="F38" s="1">
         <v>13</v>
       </c>
+      <c r="G38" s="1">
+        <v>11</v>
+      </c>
+      <c r="H38" s="1">
+        <v>537.59</v>
+      </c>
       <c r="I38" s="1">
         <v>758</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>29</v>
       </c>
@@ -1619,11 +1782,17 @@
       <c r="F39" s="1">
         <v>1</v>
       </c>
+      <c r="G39" s="1">
+        <v>1</v>
+      </c>
+      <c r="H39" s="1">
+        <v>12.06</v>
+      </c>
       <c r="I39" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>55</v>
       </c>
@@ -1642,11 +1811,17 @@
       <c r="F40" s="1">
         <v>9</v>
       </c>
+      <c r="G40" s="1">
+        <v>7</v>
+      </c>
+      <c r="H40" s="1">
+        <v>58.84</v>
+      </c>
       <c r="I40" s="1">
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>13</v>
       </c>
@@ -1665,11 +1840,17 @@
       <c r="F41" s="1">
         <v>1</v>
       </c>
+      <c r="G41" s="1">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1">
+        <v>15.04</v>
+      </c>
       <c r="I41" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>15</v>
       </c>
@@ -1688,11 +1869,17 @@
       <c r="F42" s="1">
         <v>1</v>
       </c>
+      <c r="G42" s="1">
+        <v>1</v>
+      </c>
+      <c r="H42" s="1">
+        <v>17.64</v>
+      </c>
       <c r="I42" s="1">
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>26</v>
       </c>
@@ -1711,11 +1898,17 @@
       <c r="F43" s="1">
         <v>0</v>
       </c>
+      <c r="G43" s="1">
+        <v>0</v>
+      </c>
+      <c r="H43" s="1">
+        <v>0.61</v>
+      </c>
       <c r="I43" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>49</v>
       </c>
@@ -1734,11 +1927,17 @@
       <c r="F44" s="1">
         <v>2</v>
       </c>
+      <c r="G44" s="1">
+        <v>2</v>
+      </c>
+      <c r="H44" s="1">
+        <v>64.3</v>
+      </c>
       <c r="I44" s="1">
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>4</v>
       </c>
@@ -1757,11 +1956,17 @@
       <c r="F45" s="1">
         <v>0</v>
       </c>
+      <c r="G45" s="1">
+        <v>0</v>
+      </c>
+      <c r="H45" s="1">
+        <v>13.93</v>
+      </c>
       <c r="I45" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>59</v>
       </c>
@@ -1780,11 +1985,17 @@
       <c r="F46" s="1">
         <v>2</v>
       </c>
+      <c r="G46" s="1">
+        <v>1</v>
+      </c>
+      <c r="H46" s="1">
+        <v>8.09</v>
+      </c>
       <c r="I46" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>52</v>
       </c>
@@ -1803,11 +2014,17 @@
       <c r="F47" s="1">
         <v>0</v>
       </c>
+      <c r="G47" s="1">
+        <v>0</v>
+      </c>
+      <c r="H47" s="1">
+        <v>2.02</v>
+      </c>
       <c r="I47" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>78</v>
       </c>
@@ -1827,14 +2044,16 @@
         <v>18</v>
       </c>
       <c r="G48" s="1">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="H48" s="1">
+        <v>299.02</v>
       </c>
       <c r="I48" s="1">
         <v>390</v>
       </c>
-      <c r="J48" s="1"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>47</v>
       </c>
@@ -1853,11 +2072,17 @@
       <c r="F49" s="1">
         <v>0</v>
       </c>
+      <c r="G49" s="1">
+        <v>0</v>
+      </c>
+      <c r="H49" s="1">
+        <v>9.7899999999999991</v>
+      </c>
       <c r="I49" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>25</v>
       </c>
@@ -1876,11 +2101,17 @@
       <c r="F50" s="1">
         <v>0</v>
       </c>
+      <c r="G50" s="1">
+        <v>0</v>
+      </c>
+      <c r="H50" s="1">
+        <v>14.15</v>
+      </c>
       <c r="I50" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>72</v>
       </c>
@@ -1900,16 +2131,16 @@
         <v>11</v>
       </c>
       <c r="G51" s="1">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="H51" s="1">
+        <v>252.19</v>
       </c>
       <c r="I51" s="1">
         <v>355</v>
       </c>
-      <c r="J51" s="1">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>50</v>
       </c>
@@ -1928,11 +2159,17 @@
       <c r="F52" s="1">
         <v>0</v>
       </c>
+      <c r="G52" s="1">
+        <v>0</v>
+      </c>
+      <c r="H52" s="1">
+        <v>22.18</v>
+      </c>
       <c r="I52" s="1">
         <v>31</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>17</v>
       </c>
@@ -1946,16 +2183,22 @@
         <v>1</v>
       </c>
       <c r="E53" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" s="1">
         <v>1</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0</v>
+      </c>
+      <c r="H53" s="1">
+        <v>22.65</v>
       </c>
       <c r="I53" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>44</v>
       </c>
@@ -1974,11 +2217,17 @@
       <c r="F54" s="1">
         <v>0</v>
       </c>
+      <c r="G54" s="1">
+        <v>0</v>
+      </c>
+      <c r="H54" s="1">
+        <v>11.55</v>
+      </c>
       <c r="I54" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>32</v>
       </c>
@@ -1997,11 +2246,17 @@
       <c r="F55" s="1">
         <v>0</v>
       </c>
+      <c r="G55" s="1">
+        <v>0</v>
+      </c>
+      <c r="H55" s="1">
+        <v>0.98</v>
+      </c>
       <c r="I55" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>5</v>
       </c>
@@ -2020,11 +2275,17 @@
       <c r="F56" s="1">
         <v>1</v>
       </c>
+      <c r="G56" s="1">
+        <v>0</v>
+      </c>
+      <c r="H56" s="1">
+        <v>6.19</v>
+      </c>
       <c r="I56" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>60</v>
       </c>
@@ -2043,11 +2304,17 @@
       <c r="F57" s="1">
         <v>2</v>
       </c>
+      <c r="G57" s="1">
+        <v>2</v>
+      </c>
+      <c r="H57" s="1">
+        <v>160.63999999999999</v>
+      </c>
       <c r="I57" s="1">
         <v>231</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>11</v>
       </c>
@@ -2066,11 +2333,17 @@
       <c r="F58" s="1">
         <v>0</v>
       </c>
+      <c r="G58" s="1">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1">
+        <v>35.6</v>
+      </c>
       <c r="I58" s="1">
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>50</v>
       </c>
@@ -2089,11 +2362,17 @@
       <c r="F59" s="1">
         <v>0</v>
       </c>
+      <c r="G59" s="1">
+        <v>0</v>
+      </c>
+      <c r="H59" s="1">
+        <v>5.05</v>
+      </c>
       <c r="I59" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>70</v>
       </c>
@@ -2112,11 +2391,17 @@
       <c r="F60" s="1">
         <v>6</v>
       </c>
+      <c r="G60" s="1">
+        <v>6</v>
+      </c>
+      <c r="H60" s="1">
+        <v>77.38</v>
+      </c>
       <c r="I60" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>4</v>
       </c>
@@ -2135,11 +2420,17 @@
       <c r="F61" s="1">
         <v>0</v>
       </c>
+      <c r="G61" s="1">
+        <v>0</v>
+      </c>
+      <c r="H61" s="1">
+        <v>13.43</v>
+      </c>
       <c r="I61" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>5</v>
       </c>
@@ -2158,11 +2449,17 @@
       <c r="F62" s="1">
         <v>0</v>
       </c>
+      <c r="G62" s="1">
+        <v>0</v>
+      </c>
+      <c r="H62" s="1">
+        <v>5.9</v>
+      </c>
       <c r="I62" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>20</v>
       </c>
@@ -2181,11 +2478,17 @@
       <c r="F63" s="1">
         <v>0</v>
       </c>
+      <c r="G63" s="1">
+        <v>0</v>
+      </c>
+      <c r="H63" s="1">
+        <v>4.08</v>
+      </c>
       <c r="I63" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>31</v>
       </c>
@@ -2203,6 +2506,12 @@
       </c>
       <c r="F64" s="1">
         <v>0</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0</v>
+      </c>
+      <c r="H64" s="1">
+        <v>1.26</v>
       </c>
       <c r="I64" s="1">
         <v>2</v>
@@ -2227,6 +2536,12 @@
       <c r="F65" s="1">
         <v>0</v>
       </c>
+      <c r="G65" s="1">
+        <v>0</v>
+      </c>
+      <c r="H65" s="1">
+        <v>22.63</v>
+      </c>
       <c r="I65" s="1">
         <v>32</v>
       </c>
@@ -2250,6 +2565,12 @@
       <c r="F66" s="1">
         <v>0</v>
       </c>
+      <c r="G66" s="1">
+        <v>0</v>
+      </c>
+      <c r="H66" s="1">
+        <v>91.53</v>
+      </c>
       <c r="I66" s="1">
         <v>123</v>
       </c>
@@ -2273,6 +2594,12 @@
       <c r="F67" s="1">
         <v>0</v>
       </c>
+      <c r="G67" s="1">
+        <v>0</v>
+      </c>
+      <c r="H67" s="1">
+        <v>330.26</v>
+      </c>
       <c r="I67" s="1">
         <v>430</v>
       </c>
@@ -2296,6 +2623,12 @@
       <c r="F68" s="1">
         <v>1</v>
       </c>
+      <c r="G68" s="1">
+        <v>1</v>
+      </c>
+      <c r="H68" s="1">
+        <v>31.1</v>
+      </c>
       <c r="I68" s="1">
         <v>42</v>
       </c>
@@ -2319,6 +2652,12 @@
       <c r="F69" s="1">
         <v>0</v>
       </c>
+      <c r="G69" s="1">
+        <v>0</v>
+      </c>
+      <c r="H69" s="1">
+        <v>25.32</v>
+      </c>
       <c r="I69" s="1">
         <v>36</v>
       </c>
@@ -2342,6 +2681,12 @@
       <c r="F70" s="1">
         <v>0</v>
       </c>
+      <c r="G70" s="1">
+        <v>0</v>
+      </c>
+      <c r="H70" s="1">
+        <v>7.69</v>
+      </c>
       <c r="I70" s="1">
         <v>11</v>
       </c>
@@ -2365,6 +2710,12 @@
       <c r="F71" s="1">
         <v>4</v>
       </c>
+      <c r="G71" s="1">
+        <v>1</v>
+      </c>
+      <c r="H71" s="1">
+        <v>172.92</v>
+      </c>
       <c r="I71" s="1">
         <v>238</v>
       </c>
@@ -2388,6 +2739,12 @@
       <c r="F72" s="1">
         <v>3</v>
       </c>
+      <c r="G72" s="1">
+        <v>2</v>
+      </c>
+      <c r="H72" s="1">
+        <v>125.62</v>
+      </c>
       <c r="I72" s="1">
         <v>165</v>
       </c>
@@ -2411,6 +2768,12 @@
       <c r="F73" s="1">
         <v>0</v>
       </c>
+      <c r="G73" s="1">
+        <v>0</v>
+      </c>
+      <c r="H73" s="1">
+        <v>9.93</v>
+      </c>
       <c r="I73" s="1">
         <v>13</v>
       </c>
@@ -2434,6 +2797,12 @@
       <c r="F74" s="1">
         <v>0</v>
       </c>
+      <c r="G74" s="1">
+        <v>0</v>
+      </c>
+      <c r="H74" s="1">
+        <v>2.75</v>
+      </c>
       <c r="I74" s="1">
         <v>4</v>
       </c>
@@ -2457,6 +2826,12 @@
       <c r="F75" s="1">
         <v>0</v>
       </c>
+      <c r="G75" s="1">
+        <v>0</v>
+      </c>
+      <c r="H75" s="1">
+        <v>41.18</v>
+      </c>
       <c r="I75" s="1">
         <v>57</v>
       </c>
@@ -2480,6 +2855,12 @@
       <c r="F76" s="1">
         <v>0</v>
       </c>
+      <c r="G76" s="1">
+        <v>0</v>
+      </c>
+      <c r="H76" s="1">
+        <v>1.57</v>
+      </c>
       <c r="I76" s="1">
         <v>2</v>
       </c>
@@ -2503,6 +2884,12 @@
       <c r="F77" s="1">
         <v>0</v>
       </c>
+      <c r="G77" s="1">
+        <v>0</v>
+      </c>
+      <c r="H77" s="1">
+        <v>22.37</v>
+      </c>
       <c r="I77" s="1">
         <v>31</v>
       </c>
@@ -2526,6 +2913,12 @@
       <c r="F78" s="1">
         <v>1</v>
       </c>
+      <c r="G78" s="1">
+        <v>1</v>
+      </c>
+      <c r="H78" s="1">
+        <v>121.33</v>
+      </c>
       <c r="I78" s="1">
         <v>160</v>
       </c>
@@ -2549,6 +2942,12 @@
       <c r="F79" s="1">
         <v>0</v>
       </c>
+      <c r="G79" s="1">
+        <v>0</v>
+      </c>
+      <c r="H79" s="1">
+        <v>2.91</v>
+      </c>
       <c r="I79" s="1">
         <v>4</v>
       </c>
@@ -2572,6 +2971,12 @@
       <c r="F80" s="1">
         <v>0</v>
       </c>
+      <c r="G80" s="1">
+        <v>0</v>
+      </c>
+      <c r="H80" s="1">
+        <v>59.06</v>
+      </c>
       <c r="I80" s="1">
         <v>81</v>
       </c>
@@ -2595,6 +3000,12 @@
       <c r="F81" s="1">
         <v>0</v>
       </c>
+      <c r="G81" s="1">
+        <v>0</v>
+      </c>
+      <c r="H81" s="1">
+        <v>34.47</v>
+      </c>
       <c r="I81" s="1">
         <v>45</v>
       </c>
@@ -2618,6 +3029,12 @@
       <c r="F82" s="1">
         <v>1</v>
       </c>
+      <c r="G82" s="1">
+        <v>0</v>
+      </c>
+      <c r="H82" s="1">
+        <v>35.94</v>
+      </c>
       <c r="I82" s="1">
         <v>51</v>
       </c>
@@ -2641,6 +3058,12 @@
       <c r="F83" s="1">
         <v>0</v>
       </c>
+      <c r="G83" s="1">
+        <v>0</v>
+      </c>
+      <c r="H83" s="1">
+        <v>4.55</v>
+      </c>
       <c r="I83" s="1">
         <v>6</v>
       </c>
@@ -2664,6 +3087,12 @@
       <c r="F84" s="1">
         <v>1</v>
       </c>
+      <c r="G84" s="1">
+        <v>0</v>
+      </c>
+      <c r="H84" s="1">
+        <v>4.49</v>
+      </c>
       <c r="I84" s="1">
         <v>7</v>
       </c>
@@ -2687,6 +3116,12 @@
       <c r="F85" s="1">
         <v>1</v>
       </c>
+      <c r="G85" s="1">
+        <v>1</v>
+      </c>
+      <c r="H85" s="1">
+        <v>15.47</v>
+      </c>
       <c r="I85" s="1">
         <v>20</v>
       </c>
@@ -2709,6 +3144,12 @@
       </c>
       <c r="F86" s="1">
         <v>0</v>
+      </c>
+      <c r="G86" s="1">
+        <v>0</v>
+      </c>
+      <c r="H86" s="1">
+        <v>4.57</v>
       </c>
       <c r="I86" s="1">
         <v>6</v>
@@ -2733,6 +3174,12 @@
       <c r="F87" s="1">
         <v>3</v>
       </c>
+      <c r="G87" s="1">
+        <v>2</v>
+      </c>
+      <c r="H87" s="1">
+        <v>442.89</v>
+      </c>
       <c r="I87" s="1">
         <v>614</v>
       </c>
@@ -2756,6 +3203,12 @@
       <c r="F88" s="1">
         <v>0</v>
       </c>
+      <c r="G88" s="1">
+        <v>0</v>
+      </c>
+      <c r="H88" s="1">
+        <v>43.19</v>
+      </c>
       <c r="I88" s="1">
         <v>55</v>
       </c>
@@ -2779,6 +3232,12 @@
       <c r="F89" s="1">
         <v>1</v>
       </c>
+      <c r="G89" s="1">
+        <v>1</v>
+      </c>
+      <c r="H89" s="1">
+        <v>114.2</v>
+      </c>
       <c r="I89" s="1">
         <v>156</v>
       </c>
@@ -2802,6 +3261,12 @@
       <c r="F90" s="1">
         <v>2</v>
       </c>
+      <c r="G90" s="1">
+        <v>2</v>
+      </c>
+      <c r="H90" s="1">
+        <v>77.489999999999995</v>
+      </c>
       <c r="I90" s="1">
         <v>105</v>
       </c>
@@ -2825,6 +3290,12 @@
       <c r="F91" s="1">
         <v>0</v>
       </c>
+      <c r="G91" s="1">
+        <v>0</v>
+      </c>
+      <c r="H91" s="1">
+        <v>6.37</v>
+      </c>
       <c r="I91" s="1">
         <v>8</v>
       </c>
@@ -2848,6 +3319,12 @@
       <c r="F92" s="1">
         <v>0</v>
       </c>
+      <c r="G92" s="1">
+        <v>0</v>
+      </c>
+      <c r="H92" s="1">
+        <v>14.89</v>
+      </c>
       <c r="I92" s="1">
         <v>20</v>
       </c>
@@ -2871,6 +3348,12 @@
       <c r="F93" s="1">
         <v>0</v>
       </c>
+      <c r="G93" s="1">
+        <v>0</v>
+      </c>
+      <c r="H93" s="1">
+        <v>25.9</v>
+      </c>
       <c r="I93" s="1">
         <v>34</v>
       </c>
@@ -2894,6 +3377,12 @@
       <c r="F94" s="1">
         <v>0</v>
       </c>
+      <c r="G94" s="1">
+        <v>0</v>
+      </c>
+      <c r="H94" s="1">
+        <v>29.1</v>
+      </c>
       <c r="I94" s="1">
         <v>38</v>
       </c>
@@ -2917,6 +3406,12 @@
       <c r="F95" s="1">
         <v>0</v>
       </c>
+      <c r="G95" s="1">
+        <v>0</v>
+      </c>
+      <c r="H95" s="1">
+        <v>24.44</v>
+      </c>
       <c r="I95" s="1">
         <v>34</v>
       </c>
@@ -2940,6 +3435,12 @@
       <c r="F96" s="1">
         <v>0</v>
       </c>
+      <c r="G96" s="1">
+        <v>0</v>
+      </c>
+      <c r="H96" s="1">
+        <v>18.3</v>
+      </c>
       <c r="I96" s="1">
         <v>26</v>
       </c>
@@ -2963,6 +3464,12 @@
       <c r="F97" s="1">
         <v>0</v>
       </c>
+      <c r="G97" s="1">
+        <v>0</v>
+      </c>
+      <c r="H97" s="1">
+        <v>6.9</v>
+      </c>
       <c r="I97" s="1">
         <v>10</v>
       </c>
@@ -2986,6 +3493,12 @@
       <c r="F98" s="1">
         <v>0</v>
       </c>
+      <c r="G98" s="1">
+        <v>0</v>
+      </c>
+      <c r="H98" s="1">
+        <v>26.31</v>
+      </c>
       <c r="I98" s="1">
         <v>36</v>
       </c>
@@ -3009,6 +3522,12 @@
       <c r="F99" s="1">
         <v>1</v>
       </c>
+      <c r="G99" s="1">
+        <v>0</v>
+      </c>
+      <c r="H99" s="1">
+        <v>42.8</v>
+      </c>
       <c r="I99" s="1">
         <v>56</v>
       </c>
@@ -3032,6 +3551,12 @@
       <c r="F100" s="1">
         <v>0</v>
       </c>
+      <c r="G100" s="1">
+        <v>0</v>
+      </c>
+      <c r="H100" s="1">
+        <v>4.49</v>
+      </c>
       <c r="I100" s="1">
         <v>6</v>
       </c>
@@ -3055,6 +3580,12 @@
       <c r="F101" s="1">
         <v>1</v>
       </c>
+      <c r="G101" s="1">
+        <v>0</v>
+      </c>
+      <c r="H101" s="1">
+        <v>53.01</v>
+      </c>
       <c r="I101" s="1">
         <v>69</v>
       </c>
@@ -3077,6 +3608,12 @@
       </c>
       <c r="F102" s="1">
         <v>0</v>
+      </c>
+      <c r="G102" s="1">
+        <v>0</v>
+      </c>
+      <c r="H102" s="1">
+        <v>7.45</v>
       </c>
       <c r="I102" s="1">
         <v>10</v>
@@ -3098,6 +3635,12 @@
       </c>
       <c r="F104" s="1" t="s">
         <v>107</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="I104" s="1" t="s">
         <v>109</v>
@@ -3115,12 +3658,20 @@
       </c>
       <c r="E105" s="1">
         <f>SUM(E8:E102)</f>
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F105">
         <f>SUM(F8:F102)</f>
         <v>116</v>
       </c>
+      <c r="G105">
+        <f>SUM(G8:G102)</f>
+        <v>78</v>
+      </c>
+      <c r="H105" s="1">
+        <f>SUM(H8:H102)</f>
+        <v>4898.6499999999987</v>
+      </c>
       <c r="I105">
         <f>SUM(I8:I102)</f>
         <v>6751</v>
@@ -3131,9 +3682,30 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
+      <c r="D107" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F107" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
+      <c r="D108" s="1">
+        <f>E105 / D105</f>
+        <v>0.84158415841584155</v>
+      </c>
+      <c r="E108" s="1">
+        <f>G105 / C105</f>
+        <v>0.82105263157894737</v>
+      </c>
+      <c r="F108">
+        <f>H105/C105</f>
+        <v>51.564736842105248</v>
+      </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>

</xml_diff>